<commit_message>
Added drag removal analysis and tests
</commit_message>
<xml_diff>
--- a/devanalyst/resources/simulation/Team.xlsx
+++ b/devanalyst/resources/simulation/Team.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://finastra-my.sharepoint.com/personal/alejandro_hernandez_finastra_com/Documents/Theia/Development Analytics/Data Framework/Input Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\devanalyst\devanalyst\resources\simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="196" documentId="8_{902A1CFD-0361-49BB-BEF5-D1BD02BD5D04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{581DC95D-488D-4183-8BF7-49C6B0EFA757}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B529EF2-8BD2-4F35-967B-A9FA2CE24D99}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="3" xr2:uid="{418FE2D4-9925-4944-AD55-713CC4C53F1D}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" activeTab="1" xr2:uid="{418FE2D4-9925-4944-AD55-713CC4C53F1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Dev" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,11 @@
     <sheet name="User Stories count" sheetId="3" r:id="rId3"/>
     <sheet name="Code Structure" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Dev!$A$1:$E$31</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +30,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="108">
   <si>
     <t>Mervin Lindsay  </t>
   </si>
@@ -149,9 +154,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>Bounded Context</t>
-  </si>
-  <si>
     <t>Ministry of Health</t>
   </si>
   <si>
@@ -354,13 +356,23 @@
   </si>
   <si>
     <t>For this project, only 4,000 will be touched, say. (kind of like rewriting 25% of the app - so in 4 releases you would "re-do" the app).</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Functional Area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,6 +382,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -400,16 +419,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -722,23 +744,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BB6CD2-8AF2-49C0-B945-68EBB6D7C1E9}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="22.77734375" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.46484375" customWidth="1"/>
+    <col min="3" max="3" width="17.53125" customWidth="1"/>
+    <col min="4" max="4" width="22.796875" customWidth="1"/>
+    <col min="5" max="5" width="18.86328125" customWidth="1"/>
+    <col min="6" max="6" width="20.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -749,66 +771,81 @@
         <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="E2" s="4">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="E3" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="E4" s="4">
+        <v>17500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="E5" s="4">
+        <v>17500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -819,150 +856,183 @@
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="E6" s="4">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="E7" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="E8" s="4">
+        <v>23000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="E9" s="4">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="E10" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="E11" s="4">
+        <v>17500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
         <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="E12" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
         <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="E13" s="4">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
         <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="E14" s="4">
+        <v>23000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
         <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="E15" s="4">
+        <v>17500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="E16" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -973,207 +1043,253 @@
         <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="E17" s="4">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="E18" s="4">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="E19" s="4">
+        <v>23000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="E20" s="4">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="E21" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="E22" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
         <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="E23" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
         <v>37</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="E24" s="4">
+        <v>17500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
         <v>37</v>
       </c>
       <c r="D25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="E25" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" t="s">
         <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="E26" s="4">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
         <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="E27" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
         <v>37</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="E28" s="4">
+        <v>23000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
         <v>37</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="E29" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
         <v>37</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="E30" s="4">
+        <v>17500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C31" t="s">
         <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="E31" s="4">
+        <v>20000</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:A31">
+  <autoFilter ref="A1:E31" xr:uid="{A3CABF24-70AB-4373-BD14-33FA7FBDBADB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A31">
     <sortCondition ref="A2:A31"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1185,78 +1301,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{208AC510-202C-460C-A977-8C18A2BBFB47}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.19921875" customWidth="1"/>
+    <col min="2" max="2" width="20.53125" customWidth="1"/>
+    <col min="3" max="3" width="21.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -1276,119 +1392,119 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="2" max="2" width="17.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
         <v>55</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
         <v>57</v>
       </c>
-      <c r="C4" t="s">
-        <v>88</v>
-      </c>
-      <c r="I4" t="s">
-        <v>89</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
         <v>59</v>
       </c>
-      <c r="I5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>60</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="D8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D8" t="s">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="E9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="E9" t="s">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="E10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="E10" t="s">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="E11" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="E11" t="s">
-        <v>65</v>
       </c>
       <c r="I11">
         <f>4*3*11</f>
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" t="s">
         <v>66</v>
       </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="D14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D14" t="s">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="D15" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D15" t="s">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="D16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>70</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>71</v>
       </c>
-      <c r="D18" t="s">
+      <c r="I18" t="s">
+        <v>77</v>
+      </c>
+      <c r="J18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="E19" t="s">
         <v>72</v>
-      </c>
-      <c r="I18" t="s">
-        <v>78</v>
-      </c>
-      <c r="J18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E19" t="s">
-        <v>73</v>
       </c>
       <c r="I19" s="3">
         <v>0.4</v>
@@ -1397,9 +1513,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.45">
       <c r="E20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I20" s="3">
         <v>0.3</v>
@@ -1408,12 +1524,12 @@
         <v>3</v>
       </c>
       <c r="L20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.45">
       <c r="E21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I21" s="3">
         <v>0.3</v>
@@ -1422,32 +1538,32 @@
         <v>2</v>
       </c>
       <c r="L21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.45">
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.45">
       <c r="D23" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" t="s">
         <v>85</v>
       </c>
-      <c r="G23" t="s">
-        <v>86</v>
-      </c>
       <c r="I23" s="3"/>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" t="s">
         <v>76</v>
       </c>
-      <c r="D25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.45">
       <c r="E26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I26" s="3">
         <v>0.1</v>
@@ -1456,9 +1572,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.45">
       <c r="E27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I27" s="3">
         <v>0.5</v>
@@ -1467,12 +1583,12 @@
         <v>6</v>
       </c>
       <c r="L27" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.45">
       <c r="E28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I28" s="3">
         <v>0.4</v>
@@ -1481,12 +1597,12 @@
         <v>10</v>
       </c>
       <c r="L28" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.45">
       <c r="D30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1498,83 +1614,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6662ECA5-8BCD-459A-8A18-9970F5995508}">
   <dimension ref="A2:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G3" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>